<commit_message>
Master's Projects/ Final Project - Complete
</commit_message>
<xml_diff>
--- a/Mint/data/raw/Budget Template.xlsx
+++ b/Mint/data/raw/Budget Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85769dce75e16561/Documents/04. GitHub Repository/Mint/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85769dce75e16561/Documents/04.-GitHub-Repository/Mint/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="14_{60A6D3C6-4883-4BCE-BCDC-1F67CD90F825}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FEAE57AC-82B5-4AFE-A827-AB62789CD643}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="14_{60A6D3C6-4883-4BCE-BCDC-1F67CD90F825}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{17DFBFEF-BD65-44AF-A8B3-C38843D02B1A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 Income" sheetId="9" r:id="rId1"/>
@@ -1518,7 +1518,13 @@
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0478ECBA-C54A-4981-97E9-D5F8C961F3A6}" name="TOTAL_25679" displayName="TOTAL_25679" ref="A1:Q75">
-  <autoFilter ref="A1:Q75" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <autoFilter ref="A1:Q75" xr:uid="{00000000-0009-0000-0100-000005000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Home"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{F9A172A1-FB54-4D50-A028-2BADD19B5E7A}" name="Sub-Category" totalsRowLabel="Total" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{835EA318-83FF-432E-B878-7D9922B226B9}" name="Category" dataDxfId="11"/>
@@ -4502,7 +4508,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5100,7 +5106,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5360,10 +5366,10 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>3800</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>3800</v>
+        <v>7600</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -5580,31 +5586,31 @@
         <v>250</v>
       </c>
       <c r="I9">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="Q9">
-        <v>250</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -17913,7 +17919,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
+      <selection pane="bottomRight" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17980,7 +17986,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -18008,7 +18014,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -18042,7 +18048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -18064,7 +18070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
@@ -18083,7 +18089,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -18108,10 +18114,10 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>350</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>350</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>350</v>
@@ -18138,7 +18144,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -18166,7 +18172,7 @@
         <v>-120</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>147</v>
       </c>
@@ -18197,7 +18203,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -18252,7 +18258,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -18307,7 +18313,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -18362,7 +18368,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>62</v>
       </c>
@@ -18417,7 +18423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -18472,7 +18478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>71</v>
       </c>
@@ -18527,7 +18533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>141</v>
       </c>
@@ -18582,7 +18588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>86</v>
       </c>
@@ -18601,7 +18607,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -18656,7 +18662,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>65</v>
       </c>
@@ -18675,7 +18681,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>66</v>
       </c>
@@ -18694,7 +18700,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -18713,7 +18719,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
@@ -18732,7 +18738,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>74</v>
       </c>
@@ -18751,7 +18757,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>82</v>
       </c>
@@ -18770,7 +18776,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>145</v>
       </c>
@@ -18789,7 +18795,7 @@
         <v>Input</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -18808,7 +18814,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
@@ -18827,7 +18833,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -18846,7 +18852,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -18877,7 +18883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -18896,7 +18902,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
@@ -18951,7 +18957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
@@ -19006,7 +19012,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -19061,7 +19067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -19116,7 +19122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -19171,7 +19177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>70</v>
       </c>
@@ -19276,7 +19282,7 @@
         <v>1</v>
       </c>
       <c r="J37">
-        <v>5000</v>
+        <v>1</v>
       </c>
       <c r="K37">
         <v>10000</v>
@@ -19350,10 +19356,10 @@
         <v>3300</v>
       </c>
       <c r="I39">
-        <v>3600</v>
+        <v>-1000</v>
       </c>
       <c r="J39">
-        <v>3000</v>
+        <v>4660</v>
       </c>
       <c r="K39">
         <v>-592</v>
@@ -19396,7 +19402,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>27</v>
       </c>
@@ -19451,7 +19457,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>28</v>
       </c>
@@ -19506,7 +19512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -19525,7 +19531,7 @@
         <v>Input</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>81</v>
       </c>
@@ -19580,7 +19586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>146</v>
       </c>
@@ -19599,7 +19605,7 @@
         <v>Input</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -19654,7 +19660,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>63</v>
       </c>
@@ -19709,7 +19715,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>78</v>
       </c>
@@ -19737,34 +19743,34 @@
         <v>250</v>
       </c>
       <c r="I48">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="J48">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K48">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="L48">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="M48">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="N48">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="O48">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="P48">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="Q48">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -19783,7 +19789,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>33</v>
       </c>
@@ -19838,7 +19844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>16</v>
       </c>
@@ -19887,7 +19893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>80</v>
       </c>
@@ -19906,7 +19912,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>83</v>
       </c>
@@ -19925,7 +19931,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>84</v>
       </c>
@@ -19944,7 +19950,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
@@ -19972,7 +19978,7 @@
         <v>30</v>
       </c>
       <c r="I55">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="J55">
         <v>70</v>
@@ -19999,7 +20005,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>75</v>
       </c>
@@ -20027,7 +20033,7 @@
         <v>2</v>
       </c>
       <c r="I56">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="J56">
         <v>-198</v>
@@ -20054,7 +20060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>39</v>
       </c>
@@ -20109,7 +20115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>69</v>
       </c>
@@ -20164,7 +20170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>38</v>
       </c>
@@ -20183,7 +20189,7 @@
         <v>Est</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>85</v>
       </c>
@@ -20238,7 +20244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>35</v>
       </c>
@@ -20293,7 +20299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>36</v>
       </c>
@@ -20348,7 +20354,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>92</v>
       </c>
@@ -20403,7 +20409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>46</v>
       </c>
@@ -20458,7 +20464,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>56</v>
       </c>
@@ -20477,7 +20483,7 @@
         <v>Input</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>61</v>
       </c>
@@ -20496,7 +20502,7 @@
         <v>Input</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>67</v>
       </c>
@@ -20515,7 +20521,7 @@
         <v>Input</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>34</v>
       </c>
@@ -20570,7 +20576,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>79</v>
       </c>
@@ -20625,7 +20631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>19</v>
       </c>
@@ -20680,7 +20686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>29</v>
       </c>
@@ -20699,7 +20705,7 @@
         <v>Input</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>93</v>
       </c>
@@ -20754,7 +20760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>94</v>
       </c>
@@ -20809,7 +20815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>18</v>
       </c>
@@ -20837,7 +20843,7 @@
         <v>1500</v>
       </c>
       <c r="I74">
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="J74">
         <v>1000</v>
@@ -20864,7 +20870,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>143</v>
       </c>

</xml_diff>